<commit_message>
Small text change in example files.
</commit_message>
<xml_diff>
--- a/Exempel.xlsx
+++ b/Exempel.xlsx
@@ -36,15 +36,9 @@
     <t>Grund för statlig inkomstskatt</t>
   </si>
   <si>
-    <t>Brytpunkt 1</t>
-  </si>
-  <si>
     <t>Skattesats</t>
   </si>
   <si>
-    <t>Brytpunkt 2</t>
-  </si>
-  <si>
     <t>Grund för värnskatt</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>Skattesatser</t>
+  </si>
+  <si>
+    <t>Brytpunkt för statlig inkomstskatt</t>
+  </si>
+  <si>
+    <t>Brytpunkt för värnskatt</t>
   </si>
 </sst>
 </file>
@@ -430,12 +430,12 @@
   <dimension ref="A2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -453,14 +453,14 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6">
         <v>413200</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="7">
         <v>0.2</v>
@@ -468,14 +468,14 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6">
         <v>591600</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="7">
         <v>0.05</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="4">
         <f>IF(B10&gt;$B$4,B10-$B$42,0)</f>
@@ -656,7 +656,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" ref="B15:H15" si="3">B$10*$B$21+B$11*$E$3+B$12*$E$4</f>
@@ -701,7 +701,7 @@
     </row>
     <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -719,7 +719,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" s="8">
         <v>0.33139999999999997</v>

</xml_diff>